<commit_message>
Alteração do xpath lido
</commit_message>
<xml_diff>
--- a/cnpjs.xlsx
+++ b/cnpjs.xlsx
@@ -507,6 +507,29 @@
           <t xml:space="preserve"> SP</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>94.20-1-00</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>OUTRAS ATIVIDADES DE SERVIÇOS</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>94</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>ATIVIDADES DE ORGANIZAÇÕES ASSOCIATIVAS</t>
+        </is>
+      </c>
       <c r="J2" t="inlineStr">
         <is>
           <t>ATIVIDADES DE ORGANIZAÇÕES SINDICAIS</t>
@@ -534,6 +557,34 @@
           <t xml:space="preserve"> RS</t>
         </is>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>47.11-3-02</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>COMÉRCIO; REPARAÇÃO DE VEÍCULOS AUTOMOTORES E MOTOCICLETAS</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>47</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>COMÉRCIO VAREJISTA</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>COMÉRCIO VAREJISTA DE MERCADORIAS EM GERAL, COM PREDOMINÂNCIA DE PRODUTOS ALIMENTÍCIOS - SUPERMERCADOS</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -613,6 +664,49 @@
           <t>04.353.635/0001-23</t>
         </is>
       </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>DANIEL BORGONOVO THIVES</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">JOINVILLE </t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> SC</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>56.11-2-01</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>ALOJAMENTO E ALIMENTAÇÃO</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>56</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>ALIMENTAÇÃO</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>RESTAURANTES E SIMILARES</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -620,6 +714,21 @@
           <t>19.047.351/0001-86</t>
         </is>
       </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>HP PNEUS E SERVICOS AUTOMOTIVOS LTDA</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BRASILIA </t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> DF</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -627,6 +736,49 @@
           <t>10.327.810/0001-00</t>
         </is>
       </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>M.S.M.- MINAS SERVICOS E MONTAGENS LTDA</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ITAJUBA </t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MG</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>26.32-9-00</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>INDÚSTRIAS DE TRANSFORMAÇÃO</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>26</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>FABRICAÇÃO DE EQUIPAMENTOS DE INFORMÁTICA, PRODUTOS ELETRÔNICOS E ÓPTICOS</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>FABRICAÇÃO DE APARELHOS TELEFÔNICOS E DE OUTROS EQUIPAMENTOS DE COMUNICAÇÃO, PEÇAS E ACESSÓRIOS</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -634,6 +786,21 @@
           <t>22.228.571/0001-10</t>
         </is>
       </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>IRMANDADE DA SANTA CASA DE CARIDADE DE MACHADO</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MACHADO </t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MG</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -641,6 +808,49 @@
           <t>04.121.168/0001-06</t>
         </is>
       </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>SINDICATO DOS TRABALHADORES NAS EMPRESAS DE ENERGIA DO RIO DE JANEIRO E REGIAO - SINTERGIA/RJ</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">RIO DE JANEIRO </t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> RJ</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>94.20-1-00</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>OUTRAS ATIVIDADES DE SERVIÇOS</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>94</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>ATIVIDADES DE ORGANIZAÇÕES ASSOCIATIVAS</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>ATIVIDADES DE ORGANIZAÇÕES SINDICAIS</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -648,6 +858,21 @@
           <t>29.958.609/0004-00</t>
         </is>
       </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>NIDEC GLOBAL APPLIANCE BRASIL LTDA</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ITAIOPOLIS </t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> SC</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -655,6 +880,49 @@
           <t>29.958.609/0003-11</t>
         </is>
       </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>NIDEC GLOBAL APPLIANCE BRASIL LTDA</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">JOINVILLE </t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> SC</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>24.51-2-00</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>INDÚSTRIAS DE TRANSFORMAÇÃO</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>24</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>METALURGIA</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>FUNDIÇÃO DE FERRO E AÇO</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -662,6 +930,21 @@
           <t>29.958.609/0001-50</t>
         </is>
       </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>NIDEC GLOBAL APPLIANCE BRASIL LTDA</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">JOINVILLE </t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> SC</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -669,6 +952,21 @@
           <t>90.268.723/0001-69</t>
         </is>
       </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>TUBOCANO ARTEFATOS DE CIMENTO LTDA</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GRAVATAI </t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> RS</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -676,6 +974,21 @@
           <t>82.638.644/0001-74</t>
         </is>
       </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>UNIVERSAL LEAF TABACOS LTDA</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SANTA CRUZ DO SUL </t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> RS</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -683,6 +996,21 @@
           <t>61.452.868/0001-17</t>
         </is>
       </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>PELICAN TEXTIL LTDA</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SANTA ISABEL </t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> SP</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -690,6 +1018,21 @@
           <t>19.963.333/0001-44</t>
         </is>
       </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>HERCILIO RESTAURANTE E CAFE LTDA</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">FLORIANOPOLIS </t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> SC</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -697,6 +1040,21 @@
           <t>18.810.553/0001-75</t>
         </is>
       </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>FINSOL SOCIEDADE DE CREDITO AO MICROEMPREENDEDOR E A EMPRESA DE PEQUENO PORTE S/A</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">RECIFE </t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> PE</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -704,6 +1062,49 @@
           <t>13.484.737/0001-79</t>
         </is>
       </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>RJS CONSTRUCAO CIVIL LTDA</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">FRANCISCO MORATO </t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> SP</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>41.20-4-00</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>CONSTRUÇÃO</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>41</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>CONSTRUÇÃO DE EDIFÍCIOS</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>CONSTRUÇÃO DE EDIFÍCIOS</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -711,6 +1112,21 @@
           <t>11.690.498/0001-88</t>
         </is>
       </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>CESARI ENGENHARIA E CONSTRUCAO LTDA</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BARRETOS </t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> SP</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -718,6 +1134,21 @@
           <t>26.127.417/0001-03</t>
         </is>
       </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>PECUARIA FERNANDO LTDA</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MEDIANEIRA </t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> PR</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -725,6 +1156,21 @@
           <t>01.568.077/0002-06</t>
         </is>
       </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>B-GREEN GESTAO AMBIENTAL LTDA</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">RECIFE </t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> PE</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -732,6 +1178,21 @@
           <t>24.071.686/0001-70</t>
         </is>
       </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>L &amp; R RESTAURANTE EIRELI</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAMPO GRANDE </t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MS</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -739,6 +1200,21 @@
           <t>89.896.138/0001-24</t>
         </is>
       </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>TIARAJU ENGENHARIA LTDA</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PASSO FUNDO </t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> RS</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -746,6 +1222,49 @@
           <t>30.133.029/0001-02</t>
         </is>
       </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>SIND ESTAB ENSINO NO EST DO RIO DE JANEIRO</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">NITEROI </t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> RJ</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>94.20-1-00</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>OUTRAS ATIVIDADES DE SERVIÇOS</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
+        <v>94</v>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>ATIVIDADES DE ORGANIZAÇÕES ASSOCIATIVAS</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>ATIVIDADES DE ORGANIZAÇÕES SINDICAIS</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -753,6 +1272,21 @@
           <t>62.389.168/0001-98</t>
         </is>
       </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>MATEUBRAS - COMERCIO DE MATERIAIS PARA CONSTRUCAO LTDA</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SAO PAULO </t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> SP</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -760,6 +1294,21 @@
           <t>21.878.892/0001-06</t>
         </is>
       </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>HTS ADMINISTRADORA DE HOTEIS LTDA.</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MANAUS </t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> AM</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -767,6 +1316,21 @@
           <t>92.773.142/0001-00</t>
         </is>
       </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>ASSOCIACAO SULINA DE CREDITO E ASSISTENCIA RURAL</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PORTO ALEGRE </t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> RS</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -774,6 +1338,21 @@
           <t>04.885.819/0001-34</t>
         </is>
       </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>NUTRIPURA NUTRICAO ANIMAL LTDA</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">RONDONOPOLIS </t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MT</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -781,6 +1360,49 @@
           <t>05.379.899/0001-19</t>
         </is>
       </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>SINDICATO DOS EMPRESARIOS LOTERICOS DO ESTADO DE GOIAS</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GOIANIA </t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GO</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>94.20-1-00</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>OUTRAS ATIVIDADES DE SERVIÇOS</t>
+        </is>
+      </c>
+      <c r="H30" t="n">
+        <v>94</v>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>ATIVIDADES DE ORGANIZAÇÕES ASSOCIATIVAS</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>ATIVIDADES DE ORGANIZAÇÕES SINDICAIS</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -788,6 +1410,21 @@
           <t>02.553.555/0001-96</t>
         </is>
       </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>CHT QUIMIPEL BRAZIL QUIMICA LTDA.</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PIRACAIA </t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> SP</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -795,6 +1432,21 @@
           <t>09.350.946/0001-52</t>
         </is>
       </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>CSVIVA SOLUCOES TECNICAS LTDA</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SAO CARLOS </t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> SP</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -802,11 +1454,41 @@
           <t>15.299.131/0002-70</t>
         </is>
       </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>CONSERV LOCADORA E TRANSPORTADORA LTDA</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">JACOBINA </t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> BA</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
           <t>15.299.131/0001-99</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>CONSERV LOCADORA E TRANSPORTADORA LTDA</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MARACAS </t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> BA</t>
         </is>
       </c>
     </row>

</xml_diff>